<commit_message>
Fix Global Service UUID blank
</commit_message>
<xml_diff>
--- a/lib/devdata/services/service.xlsx
+++ b/lib/devdata/services/service.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\kiry\Documents\oscar-web\lib\devdata\services\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-18.04\home\kiry\Documents\oscar-web\lib\devdata\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06D30DF-1F51-4343-8827-EE64B7F66720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21EC77E-D23E-4694-9868-A292B4BB61B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Social Work / Case Work</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Not Specified</t>
+  </si>
+  <si>
+    <t>Literacy Support</t>
   </si>
 </sst>
 </file>
@@ -324,8 +327,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -335,33 +338,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -649,16 +643,16 @@
   </sheetPr>
   <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="14.42578125" customWidth="1"/>
+    <col min="1" max="10" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,14 +686,14 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -733,10 +727,10 @@
       <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="7" t="s">
         <v>59</v>
       </c>
       <c r="N2" s="3"/>
@@ -753,7 +747,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -775,7 +769,7 @@
       <c r="G3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="I3" s="2" t="s">
@@ -784,11 +778,11 @@
       <c r="J3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="9" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M3" s="4" t="s">
         <v>61</v>
       </c>
       <c r="N3" s="3"/>
@@ -805,8 +799,8 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
+    <row r="4" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
         <v>31</v>
       </c>
@@ -834,11 +828,11 @@
       <c r="J4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="5"/>
-      <c r="L4" s="13" t="s">
+      <c r="K4" s="2"/>
+      <c r="L4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="8" t="s">
         <v>60</v>
       </c>
       <c r="N4" s="3"/>
@@ -855,12 +849,12 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+    <row r="5" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
@@ -876,15 +870,15 @@
       <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="2"/>
+      <c r="L5" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -899,25 +893,25 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
     </row>
-    <row r="6" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="4"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
@@ -933,25 +927,25 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
     </row>
-    <row r="7" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+    <row r="7" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="6"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="4"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
@@ -967,21 +961,23 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
+    <row r="8" spans="1:26" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="7"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
@@ -997,10 +993,10 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
     </row>
-    <row r="9" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -1025,7 +1021,7 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1053,7 +1049,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -1081,7 +1077,7 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>

</xml_diff>